<commit_message>
Running on operator controller.  Not tested with robot yet
</commit_message>
<xml_diff>
--- a/OperatorController/OperatorControllerIOTable.xlsx
+++ b/OperatorController/OperatorControllerIOTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DavidTurner/Dropbox/Git/2019-Robot/OperatorController/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040A55C8-39C2-894F-BC8A-A34A4F0744CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DA101D-43E8-9943-9601-5E30F13589C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10340" windowHeight="17000" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17000" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="228" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1241,11 +1241,8 @@
       <c r="E2" s="5">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
+      <c r="F2" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1283,10 +1280,12 @@
       <c r="E4" s="5">
         <v>6</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3"/>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
@@ -1556,7 +1555,7 @@
         <v>53</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
@@ -1714,7 +1713,7 @@
         <v>76</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -1809,7 +1808,7 @@
         <v>91</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
@@ -1828,7 +1827,7 @@
         <v>94</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
@@ -1847,7 +1846,7 @@
         <v>97</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
@@ -1866,7 +1865,7 @@
         <v>100</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Documented operator controller gamepad outputs and implemented stateful position buttons on operator controller
</commit_message>
<xml_diff>
--- a/OperatorController/OperatorControllerIOTable.xlsx
+++ b/OperatorController/OperatorControllerIOTable.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Pins" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="GamepadButtons" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="233">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -97,309 +98,327 @@
     <t xml:space="preserve">LED2</t>
   </si>
   <si>
+    <t xml:space="preserve">NearRocketLow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NearRocketMid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NearRocketHigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FarRocketLow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FarRocketMid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FarRocketHigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CargoShip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_Climb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button1GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_CargoHatch_Hatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rx3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_LeftRight_Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rx2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button2</t>
+  </si>
+  <si>
     <t xml:space="preserve">LowRocketNear</t>
   </si>
   <si>
-    <t xml:space="preserve">D6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED3</t>
+    <t xml:space="preserve">D18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button2GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rx1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button3</t>
   </si>
   <si>
     <t xml:space="preserve">MidRocketNear</t>
   </si>
   <si>
-    <t xml:space="preserve">D7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED4</t>
+    <t xml:space="preserve">D20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button3GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button4</t>
   </si>
   <si>
     <t xml:space="preserve">HighRocketNear</t>
   </si>
   <si>
-    <t xml:space="preserve">D8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED5</t>
+    <t xml:space="preserve">D22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button4GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_LeftRight_Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button_Unassigned1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button_Unassigned2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button_Unassigned3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button_Unassigned4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_Unassigned_1_ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_Unassigned_1_OFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_Unassigned_2_ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch_Unassigned_2_OFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unassigned1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unassigned2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unassigned3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unassigned4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button5</t>
   </si>
   <si>
     <t xml:space="preserve">LowRocketFar</t>
   </si>
   <si>
-    <t xml:space="preserve">D9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED6</t>
+    <t xml:space="preserve">D37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button5GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button6</t>
   </si>
   <si>
     <t xml:space="preserve">MidRocketFar</t>
   </si>
   <si>
-    <t xml:space="preserve">D10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED7</t>
+    <t xml:space="preserve">D39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button6GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button7</t>
   </si>
   <si>
     <t xml:space="preserve">HighRocketFar</t>
   </si>
   <si>
-    <t xml:space="preserve">D11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CargoShip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_Climb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button1GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tx3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_CargoHatch_Hatch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rx3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_LeftRight_Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tx2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rx2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tx1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button2GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rx1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button3GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button4GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_LeftRight_Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button_Unassigned1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button_Unassigned2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button_Unassigned3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button_Unassigned4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_Unassigned_1_ON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_Unassigned_1_OFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_Unassigned_2_ON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch_Unassigned_2_OFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unassigned1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unassigned2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unassigned3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unassigned4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button5GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button6GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button7</t>
-  </si>
-  <si>
     <t xml:space="preserve">D41</t>
   </si>
   <si>
@@ -662,6 +681,45 @@
   </si>
   <si>
     <t xml:space="preserve">Button22GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exclusive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stateful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FarRocketNear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cargo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch1Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch1Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch2Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch2Right</t>
   </si>
 </sst>
 </file>
@@ -934,8 +992,8 @@
   </sheetPr>
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="228" zoomScaleNormal="228" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1339,15 +1397,15 @@
         <v>62</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5" t="n">
@@ -1357,16 +1415,16 @@
         <v>6</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="5" t="n">
@@ -1376,18 +1434,18 @@
         <v>6</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="5" t="n">
@@ -1397,16 +1455,16 @@
         <v>6</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="5" t="n">
@@ -1416,15 +1474,15 @@
         <v>6</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="4"/>
@@ -1435,13 +1493,13 @@
         <v>6</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="4"/>
@@ -1452,15 +1510,15 @@
         <v>9</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="4"/>
@@ -1471,15 +1529,15 @@
         <v>9</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="4"/>
@@ -1490,15 +1548,15 @@
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="4"/>
@@ -1509,15 +1567,15 @@
         <v>9</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="4"/>
@@ -1528,15 +1586,15 @@
         <v>9</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="4"/>
@@ -1547,15 +1605,15 @@
         <v>9</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="4"/>
@@ -1566,15 +1624,15 @@
         <v>9</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="4"/>
@@ -1585,15 +1643,15 @@
         <v>9</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="4"/>
@@ -1604,15 +1662,15 @@
         <v>9</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="4"/>
@@ -1623,15 +1681,15 @@
         <v>9</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="4"/>
@@ -1642,15 +1700,15 @@
         <v>9</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="4"/>
@@ -1661,15 +1719,15 @@
         <v>9</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="4"/>
@@ -1680,15 +1738,15 @@
         <v>9</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="4"/>
@@ -1699,15 +1757,15 @@
         <v>9</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="4"/>
@@ -1718,13 +1776,13 @@
         <v>9</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="4"/>
@@ -1735,15 +1793,15 @@
         <v>9</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="4"/>
@@ -1754,13 +1812,13 @@
         <v>9</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="G41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="4"/>
@@ -1771,15 +1829,15 @@
         <v>9</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="4"/>
@@ -1790,13 +1848,13 @@
         <v>9</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="G43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="4"/>
@@ -1807,7 +1865,7 @@
         <v>9</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>43</v>
@@ -1815,7 +1873,7 @@
     </row>
     <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="4"/>
@@ -1826,13 +1884,13 @@
         <v>6</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="4"/>
@@ -1843,15 +1901,15 @@
         <v>9</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="4"/>
@@ -1862,13 +1920,13 @@
         <v>9</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="4"/>
@@ -1879,7 +1937,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>46</v>
@@ -1887,7 +1945,7 @@
     </row>
     <row r="49" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="4"/>
@@ -1898,13 +1956,13 @@
         <v>9</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="4"/>
@@ -1915,15 +1973,15 @@
         <v>9</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="4"/>
@@ -1934,13 +1992,13 @@
         <v>9</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="4"/>
@@ -1951,15 +2009,15 @@
         <v>9</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="4"/>
@@ -1970,13 +2028,13 @@
         <v>9</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="G53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="4"/>
@@ -1987,15 +2045,15 @@
         <v>6</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="4"/>
@@ -2006,16 +2064,16 @@
         <v>9</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="5" t="n">
@@ -2025,18 +2083,18 @@
         <v>6</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="5" t="n">
@@ -2046,16 +2104,16 @@
         <v>6</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="G57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="5" t="n">
@@ -2065,18 +2123,18 @@
         <v>6</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="5" t="n">
@@ -2086,16 +2144,16 @@
         <v>6</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="G59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="5" t="n">
@@ -2105,18 +2163,18 @@
         <v>6</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="5" t="n">
@@ -2126,16 +2184,16 @@
         <v>6</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="5" t="n">
@@ -2145,18 +2203,18 @@
         <v>6</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="5" t="n">
@@ -2166,16 +2224,16 @@
         <v>6</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="G63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="5" t="n">
@@ -2185,7 +2243,7 @@
         <v>6</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>19</v>
@@ -2193,10 +2251,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="5" t="n">
@@ -2206,16 +2264,16 @@
         <v>6</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="5" t="n">
@@ -2225,18 +2283,18 @@
         <v>6</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="5" t="n">
@@ -2246,16 +2304,16 @@
         <v>6</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="G67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="5" t="n">
@@ -2265,18 +2323,18 @@
         <v>6</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="5" t="n">
@@ -2286,16 +2344,16 @@
         <v>6</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="G69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="5" t="n">
@@ -2305,18 +2363,18 @@
         <v>6</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="6" t="n">
@@ -2326,16 +2384,16 @@
         <v>9</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="6" t="n">
@@ -2345,18 +2403,18 @@
         <v>9</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="5" t="n">
@@ -2366,7 +2424,7 @@
         <v>6</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="G73" s="3"/>
     </row>
@@ -2379,4 +2437,279 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>